<commit_message>
Final Project second upload
</commit_message>
<xml_diff>
--- a/p7/Final+Project+Results.xlsx
+++ b/p7/Final+Project+Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71">
   <si>
     <t>Date</t>
   </si>
@@ -38,6 +38,9 @@
     <t>pay/click</t>
   </si>
   <si>
+    <t>Clicks/Pageviews</t>
+  </si>
+  <si>
     <t>enroll/clicks</t>
   </si>
   <si>
@@ -206,10 +209,13 @@
     <t>p3</t>
   </si>
   <si>
+    <t>点击概率</t>
+  </si>
+  <si>
+    <t>observe</t>
+  </si>
+  <si>
     <t>number of  cookies</t>
-  </si>
-  <si>
-    <t>observe</t>
   </si>
   <si>
     <t>low</t>
@@ -229,12 +235,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -247,34 +253,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -284,9 +266,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,21 +304,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,6 +321,29 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,47 +358,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -397,6 +379,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -407,7 +419,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,43 +551,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,25 +563,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,85 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,45 +610,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -651,26 +624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,166 +646,226 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1168,17 +1181,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" ht="12.75" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,19 +1214,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -1224,10 +1237,13 @@
       <c r="O1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" spans="1:14">
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>7723</v>
@@ -1249,34 +1265,38 @@
         <f>E2/C2</f>
         <v>0.101892285298399</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
+        <f>C2/B2</f>
+        <v>0.0889550692735983</v>
+      </c>
+      <c r="I2" s="2">
         <v>7716</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>686</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>105</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>34</v>
       </c>
-      <c r="L2">
-        <f>J2/I2</f>
+      <c r="M2">
+        <f>K2/J2</f>
         <v>0.153061224489796</v>
       </c>
-      <c r="M2">
-        <f>L2-F2</f>
-        <v>-0.0419897216528533</v>
-      </c>
       <c r="N2">
-        <f>K2/I2</f>
+        <f>M2-F2</f>
+        <v>-0.0419897216528531</v>
+      </c>
+      <c r="O2">
+        <f>L2/J2</f>
         <v>0.0495626822157434</v>
       </c>
     </row>
-    <row r="3" ht="12.75" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>9102</v>
@@ -1298,34 +1318,38 @@
         <f t="shared" ref="G3:G24" si="1">E3/C3</f>
         <v>0.0898587933247754</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H38" si="2">C3/B3</f>
+        <v>0.0855855855855856</v>
+      </c>
+      <c r="I3" s="2">
         <v>9288</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>785</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>116</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>91</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L24" si="2">J3/I3</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M24" si="3">K3/J3</f>
         <v>0.147770700636943</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M24" si="3">L3-F3</f>
-        <v>-0.0409327653450856</v>
-      </c>
       <c r="N3">
-        <f t="shared" ref="N3:N24" si="4">K3/I3</f>
+        <f t="shared" ref="N3:N24" si="4">M3-F3</f>
+        <v>-0.0409327653450853</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O24" si="5">L3/J3</f>
         <v>0.115923566878981</v>
       </c>
     </row>
-    <row r="4" ht="12.75" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>10511</v>
@@ -1347,34 +1371,38 @@
         <f t="shared" si="1"/>
         <v>0.104510451045105</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0864808296070783</v>
+      </c>
+      <c r="I4" s="2">
         <v>10480</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>884</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>145</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>79</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.164027149321267</v>
       </c>
       <c r="M4">
         <f t="shared" si="3"/>
-        <v>-0.0196912225159168</v>
+        <v>0.164027149321267</v>
       </c>
       <c r="N4">
         <f t="shared" si="4"/>
+        <v>-0.019691222515917</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
         <v>0.0893665158371041</v>
       </c>
     </row>
-    <row r="5" ht="12.75" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>9871</v>
@@ -1396,38 +1424,42 @@
         <f t="shared" si="1"/>
         <v>0.125598086124402</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0846925336845304</v>
+      </c>
+      <c r="I5" s="2">
         <v>9867</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>827</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>138</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>92</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>0.166868198307134</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>-0.0197346725062629</v>
+        <v>0.166868198307134</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
+        <v>-0.0197346725062628</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
         <v>0.111245465538089</v>
       </c>
-      <c r="O5">
-        <f>N2-G2</f>
-        <v>-0.0523296030826554</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" spans="1:15">
+      <c r="P5">
+        <f>O2-G2</f>
+        <v>-0.0523296030826556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>10014</v>
@@ -1449,38 +1481,42 @@
         <f t="shared" si="1"/>
         <v>0.0764635603345281</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0835829838226483</v>
+      </c>
+      <c r="I6" s="2">
         <v>9793</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>832</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>140</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>94</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>0.168269230769231</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>-0.0264738994577704</v>
+        <v>0.168269230769231</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
+        <v>-0.0264738994577702</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
         <v>0.112980769230769</v>
       </c>
-      <c r="O6">
-        <f t="shared" ref="O6:O24" si="5">N3-G3</f>
+      <c r="P6">
+        <f t="shared" ref="P6:P24" si="6">O3-G3</f>
         <v>0.0260647735542055</v>
       </c>
     </row>
-    <row r="7" ht="12.75" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>9670</v>
@@ -1502,38 +1538,42 @@
         <f t="shared" si="1"/>
         <v>0.0996354799513973</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0851085832471562</v>
+      </c>
+      <c r="I7" s="2">
         <v>9500</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>788</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>129</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>61</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>0.163705583756345</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>-0.00397363860088448</v>
+        <v>0.163705583756345</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>0.0774111675126904</v>
+        <v>-0.00397363860088484</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>-0.0151439352080004</v>
-      </c>
-    </row>
-    <row r="8" ht="12.75" spans="1:15">
+        <v>0.0774111675126904</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>-0.0151439352080009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>9008</v>
@@ -1555,38 +1595,42 @@
         <f t="shared" si="1"/>
         <v>0.101604278074866</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0830373001776199</v>
+      </c>
+      <c r="I8" s="2">
         <v>9088</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>780</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>127</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>44</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>0.162820512820513</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>-0.0323666529548882</v>
+        <v>0.162820512820513</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
-        <v>0.0564102564102564</v>
+        <v>-0.0323666529548882</v>
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>-0.0143526205863124</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" spans="1:15">
+        <v>0.0564102564102564</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>-0.0143526205863125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>7434</v>
@@ -1608,38 +1652,42 @@
         <f t="shared" si="1"/>
         <v>0.110759493670886</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0850147968792037</v>
+      </c>
+      <c r="I9" s="2">
         <v>7664</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>652</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>94</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>62</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.144171779141104</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>-0.0298788537702881</v>
+        <v>0.144171779141104</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>0.0950920245398773</v>
+        <v>-0.0298788537702877</v>
       </c>
       <c r="O9">
         <f t="shared" si="5"/>
-        <v>0.0365172088962412</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75" spans="1:15">
+        <v>0.0950920245398773</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>0.0365172088962411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>8459</v>
@@ -1661,38 +1709,42 @@
         <f t="shared" si="1"/>
         <v>0.0868306801736614</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0816881428064783</v>
+      </c>
+      <c r="I10" s="2">
         <v>8434</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>697</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>120</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>77</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0.172166427546628</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>-0.0174138908325322</v>
+        <v>0.172166427546628</v>
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>0.110473457675753</v>
+        <v>-0.0174138908325326</v>
       </c>
       <c r="O10">
         <f t="shared" si="5"/>
-        <v>-0.022224312438707</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75" spans="1:15">
+        <v>0.110473457675753</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>-0.0222243124387069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>10667</v>
@@ -1714,38 +1766,42 @@
         <f t="shared" si="1"/>
         <v>0.112659698025552</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0807162276178869</v>
+      </c>
+      <c r="I11" s="2">
         <v>10496</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>860</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>153</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>98</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.177906976744186</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>-0.0137306539178349</v>
+        <v>0.177906976744186</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>0.113953488372093</v>
+        <v>-0.013730653917835</v>
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
-        <v>-0.0451940216646099</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" spans="1:15">
+        <v>0.113953488372093</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>-0.0451940216646096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>10660</v>
@@ -1767,38 +1823,42 @@
         <f t="shared" si="1"/>
         <v>0.121107266435986</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0813320825515947</v>
+      </c>
+      <c r="I12" s="2">
         <v>10551</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>864</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>143</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>71</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0.165509259259259</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>-0.0605576380879149</v>
+        <v>0.165509259259259</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>0.0821759259259259</v>
+        <v>-0.0605576380879147</v>
       </c>
       <c r="O12">
         <f t="shared" si="5"/>
-        <v>-0.0156674691310088</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" spans="1:15">
+        <v>0.0821759259259259</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>-0.0156674691310087</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>9947</v>
@@ -1820,38 +1880,42 @@
         <f t="shared" si="1"/>
         <v>0.109785202863962</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0842465064843671</v>
+      </c>
+      <c r="I13" s="2">
         <v>9737</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>801</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>128</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>70</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0.15980024968789</v>
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>-0.0335171727464774</v>
+        <v>0.15980024968789</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>0.0873907615480649</v>
+        <v>-0.0335171727464779</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0.0236427775020919</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" spans="1:15">
+        <v>0.0873907615480649</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>0.0236427775020918</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>8324</v>
@@ -1873,38 +1937,42 @@
         <f t="shared" si="1"/>
         <v>0.0842105263157895</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.079889476213359</v>
+      </c>
+      <c r="I14" s="2">
         <v>8176</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>642</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>122</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>68</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0.190031152647975</v>
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
-        <v>-0.00094629096104748</v>
+        <v>0.190031152647975</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>0.105919003115265</v>
+        <v>-0.000946290961047924</v>
       </c>
       <c r="O14">
         <f t="shared" si="5"/>
-        <v>0.00129379034654134</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" spans="1:15">
+        <v>0.105919003115265</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="6"/>
+        <v>0.00129379034654103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>9434</v>
@@ -1926,38 +1994,42 @@
         <f t="shared" si="1"/>
         <v>0.181277860326894</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0713377146491414</v>
+      </c>
+      <c r="I15" s="2">
         <v>9402</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>697</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>194</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>94</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>0.278335724533716</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>-0.0485587776951102</v>
+        <v>0.278335724533716</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>0.134863701578192</v>
+        <v>-0.0485587776951101</v>
       </c>
       <c r="O15">
         <f t="shared" si="5"/>
-        <v>-0.0389313405100602</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" spans="1:15">
+        <v>0.134863701578192</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="6"/>
+        <v>-0.0389313405100601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <v>8687</v>
@@ -1979,38 +2051,42 @@
         <f t="shared" si="1"/>
         <v>0.185238784370478</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0795441464256936</v>
+      </c>
+      <c r="I16" s="2">
         <v>8669</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>669</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>127</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>81</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>0.1898355754858</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
-        <v>-0.0648677530236069</v>
+        <v>0.1898355754858</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>0.121076233183857</v>
+        <v>-0.0648677530236073</v>
       </c>
       <c r="O16">
         <f t="shared" si="5"/>
-        <v>-0.0223944413158969</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" spans="1:15">
+        <v>0.121076233183857</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>-0.0223944413158971</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>8896</v>
@@ -2032,38 +2108,42 @@
         <f t="shared" si="1"/>
         <v>0.146892655367232</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0795863309352518</v>
+      </c>
+      <c r="I17" s="2">
         <v>8881</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>693</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>153</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>101</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>0.220779220779221</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>-0.00662190916428204</v>
+        <v>0.220779220779221</v>
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>0.145743145743146</v>
+        <v>-0.00662190916428224</v>
       </c>
       <c r="O17">
         <f t="shared" si="5"/>
+        <v>0.145743145743146</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
         <v>0.0217084767994753</v>
       </c>
     </row>
-    <row r="18" ht="12.75" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>9535</v>
@@ -2085,38 +2165,42 @@
         <f t="shared" si="1"/>
         <v>0.163372859025033</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0796014682747771</v>
+      </c>
+      <c r="I18" s="2">
         <v>9655</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>771</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>213</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>119</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0.276264591439689</v>
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
-        <v>-0.0307182807605748</v>
+        <v>0.276264591439689</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>0.154345006485084</v>
+        <v>-0.0307182807605743</v>
       </c>
       <c r="O18">
         <f t="shared" si="5"/>
-        <v>-0.0464141587487023</v>
-      </c>
-    </row>
-    <row r="19" ht="12.75" spans="1:15">
+        <v>0.154345006485084</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>-0.0464141587487018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>9363</v>
@@ -2138,38 +2222,42 @@
         <f t="shared" si="1"/>
         <v>0.123641304347826</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0786072839901741</v>
+      </c>
+      <c r="I19" s="2">
         <v>9396</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>736</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>162</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>120</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="2"/>
-        <v>0.220108695652174</v>
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
-        <v>0.0108695652173913</v>
+        <v>0.220108695652174</v>
       </c>
       <c r="N19">
         <f t="shared" si="4"/>
-        <v>0.16304347826087</v>
+        <v>0.0108695652173909</v>
       </c>
       <c r="O19">
         <f t="shared" si="5"/>
-        <v>-0.064162551186621</v>
-      </c>
-    </row>
-    <row r="20" ht="12.75" spans="1:15">
+        <v>0.16304347826087</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="6"/>
+        <v>-0.0641625511866215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>9327</v>
@@ -2191,38 +2279,42 @@
         <f t="shared" si="1"/>
         <v>0.11637347767253</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0792323362281548</v>
+      </c>
+      <c r="I20" s="2">
         <v>9262</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>727</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>201</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>96</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>0.276478679504814</v>
       </c>
       <c r="M20">
         <f t="shared" si="3"/>
-        <v>0.0112554048092798</v>
+        <v>0.276478679504814</v>
       </c>
       <c r="N20">
         <f t="shared" si="4"/>
-        <v>0.132049518569464</v>
+        <v>0.0112554048092793</v>
       </c>
       <c r="O20">
         <f t="shared" si="5"/>
-        <v>-0.00114950962408591</v>
-      </c>
-    </row>
-    <row r="21" ht="12.75" spans="1:15">
+        <v>0.132049518569464</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="6"/>
+        <v>-0.00114950962408628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
         <v>9345</v>
@@ -2244,38 +2336,42 @@
         <f t="shared" si="1"/>
         <v>0.102179836512262</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0785446762974853</v>
+      </c>
+      <c r="I21" s="2">
         <v>9308</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>728</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>207</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>67</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>0.284340659340659</v>
       </c>
       <c r="M21">
         <f t="shared" si="3"/>
-        <v>0.0568202233733569</v>
+        <v>0.284340659340659</v>
       </c>
       <c r="N21">
         <f t="shared" si="4"/>
-        <v>0.092032967032967</v>
+        <v>0.0568202233733573</v>
       </c>
       <c r="O21">
         <f t="shared" si="5"/>
-        <v>-0.00902785253994862</v>
-      </c>
-    </row>
-    <row r="22" ht="12.75" spans="1:15">
+        <v>0.092032967032967</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="6"/>
+        <v>-0.0090278525399487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
         <v>8890</v>
@@ -2297,38 +2393,42 @@
         <f t="shared" si="1"/>
         <v>0.143059490084986</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0794150731158605</v>
+      </c>
+      <c r="I22" s="2">
         <v>8715</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>722</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>182</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>123</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>0.25207756232687</v>
       </c>
       <c r="M22">
         <f t="shared" si="3"/>
-        <v>0.00561863881412192</v>
+        <v>0.25207756232687</v>
       </c>
       <c r="N22">
         <f t="shared" si="4"/>
-        <v>0.170360110803324</v>
+        <v>0.00561863881412178</v>
       </c>
       <c r="O22">
         <f t="shared" si="5"/>
-        <v>0.0394021739130435</v>
-      </c>
-    </row>
-    <row r="23" ht="12.75" spans="1:15">
+        <v>0.170360110803324</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="6"/>
+        <v>0.0394021739130436</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2">
         <v>8460</v>
@@ -2350,38 +2450,42 @@
         <f t="shared" si="1"/>
         <v>0.136563876651982</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0804964539007092</v>
+      </c>
+      <c r="I23" s="2">
         <v>8448</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>695</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>142</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>100</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>0.20431654676259</v>
       </c>
       <c r="M23">
         <f t="shared" si="3"/>
-        <v>-0.0247583431052515</v>
+        <v>0.20431654676259</v>
       </c>
       <c r="N23">
         <f t="shared" si="4"/>
-        <v>0.143884892086331</v>
+        <v>-0.0247583431052511</v>
       </c>
       <c r="O23">
         <f t="shared" si="5"/>
-        <v>0.0156760408969331</v>
-      </c>
-    </row>
-    <row r="24" ht="12.75" spans="1:15">
+        <v>0.143884892086331</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="6"/>
+        <v>0.0156760408969335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2">
         <v>8836</v>
@@ -2403,38 +2507,42 @@
         <f t="shared" si="1"/>
         <v>0.0966810966810967</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0784291534631055</v>
+      </c>
+      <c r="I24" s="2">
         <v>8836</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>724</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>182</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>103</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="2"/>
-        <v>0.251381215469613</v>
       </c>
       <c r="M24">
         <f t="shared" si="3"/>
-        <v>-0.045877081788684</v>
+        <v>0.251381215469613</v>
       </c>
       <c r="N24">
         <f t="shared" si="4"/>
-        <v>0.142265193370166</v>
+        <v>-0.0458770817886837</v>
       </c>
       <c r="O24">
         <f t="shared" si="5"/>
-        <v>-0.0101468694792945</v>
-      </c>
-    </row>
-    <row r="25" ht="12.75" spans="1:11">
+        <v>0.142265193370166</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="6"/>
+        <v>-0.010146869479295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>9437</v>
@@ -2445,18 +2553,22 @@
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0835011126417294</v>
+      </c>
+      <c r="I25" s="2">
         <v>9359</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>789</v>
       </c>
-      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-    </row>
-    <row r="26" ht="12.75" spans="1:11">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>9420</v>
@@ -2467,18 +2579,22 @@
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0829087048832272</v>
+      </c>
+      <c r="I26" s="2">
         <v>9427</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>743</v>
       </c>
-      <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-    </row>
-    <row r="27" ht="12.75" spans="1:13">
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2">
         <v>9570</v>
@@ -2489,27 +2605,31 @@
       <c r="D27" s="1"/>
       <c r="E27" s="3"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0841170323928945</v>
+      </c>
+      <c r="I27" s="2">
         <v>9633</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>808</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="K27" s="3"/>
+      <c r="L27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M27">
-        <f>AVERAGE(M2:M24)</f>
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27">
+        <f>AVERAGE(N2:N24)</f>
         <v>-0.0207845820292659</v>
       </c>
     </row>
-    <row r="28" ht="12.75" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2">
         <v>9921</v>
@@ -2520,25 +2640,29 @@
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.083660921278097</v>
+      </c>
+      <c r="I28" s="2">
         <v>9842</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>831</v>
       </c>
-      <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28">
-        <f>STDEV(M2:M24)</f>
-        <v>0.0269646409706783</v>
-      </c>
-    </row>
-    <row r="29" ht="12.75" spans="1:13">
+      <c r="L28" s="3"/>
+      <c r="M28" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28">
+        <f>STDEV(N2:N24)</f>
+        <v>0.0269646409706782</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
         <v>9424</v>
@@ -2549,25 +2673,29 @@
       <c r="D29" s="1"/>
       <c r="E29" s="3"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0828735144312394</v>
+      </c>
+      <c r="I29" s="2">
         <v>9272</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>767</v>
       </c>
-      <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" t="s">
-        <v>42</v>
-      </c>
-      <c r="M29">
-        <f>1.96*M28</f>
-        <v>0.0528506963025295</v>
-      </c>
-    </row>
-    <row r="30" ht="12.75" spans="1:13">
+      <c r="L29" s="3"/>
+      <c r="M29" t="s">
+        <v>43</v>
+      </c>
+      <c r="N29">
+        <f>1.96*N28</f>
+        <v>0.0528506963025294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2">
         <v>9010</v>
@@ -2578,25 +2706,29 @@
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0839067702552719</v>
+      </c>
+      <c r="I30" s="2">
         <v>8969</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>760</v>
       </c>
-      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" t="s">
-        <v>44</v>
-      </c>
-      <c r="M30">
-        <f>M27-M29</f>
-        <v>-0.0736352783317954</v>
-      </c>
-    </row>
-    <row r="31" ht="12.75" spans="1:13">
+      <c r="L30" s="3"/>
+      <c r="M30" t="s">
+        <v>45</v>
+      </c>
+      <c r="N30">
+        <f>N27-N29</f>
+        <v>-0.0736352783317953</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2">
         <v>9656</v>
@@ -2607,25 +2739,29 @@
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0854391052195526</v>
+      </c>
+      <c r="I31" s="2">
         <v>9697</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>850</v>
       </c>
-      <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" t="s">
-        <v>46</v>
-      </c>
-      <c r="M31">
-        <f>M27+M29</f>
-        <v>0.0320661142732636</v>
-      </c>
-    </row>
-    <row r="32" ht="12.75" spans="1:11">
+      <c r="L31" s="3"/>
+      <c r="M31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N31">
+        <f>N27+N29</f>
+        <v>0.0320661142732634</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2">
         <v>10419</v>
@@ -2636,18 +2772,22 @@
       <c r="D32" s="1"/>
       <c r="E32" s="3"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0838852097130243</v>
+      </c>
+      <c r="I32" s="2">
         <v>10445</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>851</v>
       </c>
-      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-    </row>
-    <row r="33" ht="12.75" spans="1:11">
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2">
         <v>9880</v>
@@ -2658,18 +2798,22 @@
       <c r="D33" s="1"/>
       <c r="E33" s="3"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0840080971659919</v>
+      </c>
+      <c r="I33" s="2">
         <v>9931</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>831</v>
       </c>
-      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-    </row>
-    <row r="34" ht="12.75" spans="1:13">
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="2">
         <v>10134</v>
@@ -2680,27 +2824,31 @@
       <c r="D34" s="1"/>
       <c r="E34" s="3"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0790408525754885</v>
+      </c>
+      <c r="I34" s="2">
         <v>10042</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>802</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L34" t="s">
-        <v>38</v>
-      </c>
-      <c r="M34">
-        <f>AVERAGE(O2:O24)</f>
-        <v>-0.00964167218036858</v>
-      </c>
-    </row>
-    <row r="35" ht="12.75" spans="1:13">
+      <c r="K34" s="3"/>
+      <c r="L34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34">
+        <f>AVERAGE(P2:P24)</f>
+        <v>-0.00964167218036863</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2">
         <v>9717</v>
@@ -2711,25 +2859,29 @@
       <c r="D35" s="1"/>
       <c r="E35" s="3"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="2">
+      <c r="H35" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0837707111248328</v>
+      </c>
+      <c r="I35" s="2">
         <v>9721</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>829</v>
       </c>
-      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35">
-        <f>STDEV(O2:O24)</f>
+      <c r="L35" s="3"/>
+      <c r="M35" t="s">
+        <v>41</v>
+      </c>
+      <c r="N35">
+        <f>STDEV(P2:P24)</f>
         <v>0.0302737400577862</v>
       </c>
     </row>
-    <row r="36" ht="12.75" spans="1:13">
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2">
         <v>9192</v>
@@ -2740,25 +2892,29 @@
       <c r="D36" s="1"/>
       <c r="E36" s="3"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="2">
+      <c r="H36" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0799608355091384</v>
+      </c>
+      <c r="I36" s="2">
         <v>9304</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>770</v>
       </c>
-      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" t="s">
-        <v>42</v>
-      </c>
-      <c r="M36">
-        <f>1.96*M35</f>
+      <c r="L36" s="3"/>
+      <c r="M36" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36">
+        <f>1.96*N35</f>
         <v>0.059336530513261</v>
       </c>
     </row>
-    <row r="37" ht="12.75" spans="1:13">
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2">
         <v>8630</v>
@@ -2769,25 +2925,29 @@
       <c r="D37" s="1"/>
       <c r="E37" s="3"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="2">
+      <c r="H37" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0860950173812283</v>
+      </c>
+      <c r="I37" s="2">
         <v>8668</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>724</v>
       </c>
-      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" t="s">
-        <v>44</v>
-      </c>
-      <c r="M37">
-        <f>M34-M35</f>
+      <c r="L37" s="3"/>
+      <c r="M37" t="s">
+        <v>45</v>
+      </c>
+      <c r="N37">
+        <f>N34-N35</f>
         <v>-0.0399154122381548</v>
       </c>
     </row>
-    <row r="38" ht="12.75" spans="1:13">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2">
         <v>8970</v>
@@ -2798,23 +2958,27 @@
       <c r="D38" s="1"/>
       <c r="E38" s="3"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
+        <f t="shared" si="2"/>
+        <v>0.0804905239687848</v>
+      </c>
+      <c r="I38" s="2">
         <v>8988</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>710</v>
       </c>
-      <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" t="s">
-        <v>46</v>
-      </c>
-      <c r="M38">
-        <f>M34+M35</f>
+      <c r="L38" s="3"/>
+      <c r="M38" t="s">
+        <v>47</v>
+      </c>
+      <c r="N38">
+        <f>N34+N35</f>
         <v>0.0206320678774176</v>
       </c>
     </row>
-    <row r="39" ht="12.75" spans="1:5">
+    <row r="39" spans="1:5">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2828,9 +2992,9 @@
       <c r="D40" s="1"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" customHeight="1" spans="1:5">
+    <row r="41" customHeight="1" spans="1:8">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <f>SUM(B2:B38)</f>
@@ -2848,10 +3012,14 @@
         <f>SUM(E2:E24)</f>
         <v>2033</v>
       </c>
+      <c r="H41">
+        <f>C2/B2</f>
+        <v>0.0889550692735983</v>
+      </c>
     </row>
     <row r="42" customHeight="1" spans="2:3">
       <c r="B42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C42">
         <f>SUM(C2:C24)</f>
@@ -2860,7 +3028,7 @@
     </row>
     <row r="43" customHeight="1" spans="2:3">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43">
         <f>(D41+Experiment!D41)/(C42+Experiment!C42)</f>
@@ -2869,7 +3037,7 @@
     </row>
     <row r="44" customHeight="1" spans="2:3">
       <c r="B44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C44">
         <f>SQRT(C43*(1-C43)*(1/C42+1/Experiment!C42))</f>
@@ -2878,7 +3046,7 @@
     </row>
     <row r="45" customHeight="1" spans="2:3">
       <c r="B45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45">
         <f>1.96*C44</f>
@@ -2887,7 +3055,7 @@
     </row>
     <row r="46" customHeight="1" spans="2:3">
       <c r="B46" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C46">
         <f>G47-C45</f>
@@ -2896,14 +3064,14 @@
     </row>
     <row r="47" customHeight="1" spans="2:7">
       <c r="B47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C47">
         <f>G47+C45</f>
         <v>-0.0119863908253187</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G47">
         <f>3423/17260-3785/17293</f>
@@ -2912,14 +3080,14 @@
     </row>
     <row r="50" customHeight="1" spans="2:7">
       <c r="B50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C50">
         <f>(E41+Experiment!E41)/(C42+Experiment!C42)</f>
         <v>0.115127485312419</v>
       </c>
       <c r="F50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G50">
         <f>1945/17260-2033/17293</f>
@@ -2928,7 +3096,7 @@
     </row>
     <row r="51" customHeight="1" spans="2:3">
       <c r="B51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51">
         <f>SQRT(C50*(1-C50)*(1/C42+1/Experiment!C42))</f>
@@ -2937,7 +3105,7 @@
     </row>
     <row r="52" customHeight="1" spans="2:3">
       <c r="B52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C52">
         <f>1.96*C51</f>
@@ -2946,7 +3114,7 @@
     </row>
     <row r="53" customHeight="1" spans="2:3">
       <c r="B53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C53">
         <f>G50-C52</f>
@@ -2955,7 +3123,7 @@
     </row>
     <row r="54" customHeight="1" spans="2:3">
       <c r="B54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C54">
         <f>G50+C52</f>
@@ -2964,7 +3132,7 @@
     </row>
     <row r="56" customHeight="1" spans="2:3">
       <c r="B56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <f>(E41+Experiment!E41)/(D41+Experiment!D41)</f>
@@ -2973,7 +3141,7 @@
     </row>
     <row r="57" customHeight="1" spans="2:3">
       <c r="B57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <f>SQRT(C56*(1-C56)*(1/D41+1/Experiment!D41))</f>
@@ -2982,7 +3150,7 @@
     </row>
     <row r="58" customHeight="1" spans="2:3">
       <c r="B58" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C58">
         <f>1.96*C57</f>
@@ -2991,7 +3159,7 @@
     </row>
     <row r="59" customHeight="1" spans="2:3">
       <c r="B59" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C59">
         <f>G50-C58</f>
@@ -3000,33 +3168,55 @@
     </row>
     <row r="60" customHeight="1" spans="2:3">
       <c r="B60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C60">
         <f>G50+C58</f>
         <v>0.0181166463045786</v>
       </c>
     </row>
-    <row r="75" customHeight="1" spans="1:3">
+    <row r="74" customHeight="1" spans="6:8">
+      <c r="F74" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" customHeight="1" spans="1:7">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" customHeight="1" spans="1:2">
+        <v>65</v>
+      </c>
+      <c r="F75" t="s">
+        <v>58</v>
+      </c>
+      <c r="G75">
+        <f>(C41+Experiment!C41)/(B41+Experiment!B41)</f>
+        <v>0.0821540908978953</v>
+      </c>
+    </row>
+    <row r="76" customHeight="1" spans="1:7">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B76">
         <f>SQRT(0.5*0.5/(B41+344660))</f>
         <v>0.000601840740294325</v>
       </c>
-    </row>
-    <row r="77" customHeight="1" spans="1:3">
+      <c r="F76" t="s">
+        <v>41</v>
+      </c>
+      <c r="G76">
+        <f>SQRT(G75*(1-G75)*(1/B41+1/Experiment!B41))</f>
+        <v>0.000661060815638722</v>
+      </c>
+    </row>
+    <row r="77" customHeight="1" spans="1:8">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B77">
         <f>1.96*B76</f>
@@ -3036,33 +3226,58 @@
         <f>B41/(B41+Experiment!B41)</f>
         <v>0.500639666880613</v>
       </c>
-    </row>
-    <row r="78" customHeight="1" spans="1:2">
+      <c r="F77" t="s">
+        <v>43</v>
+      </c>
+      <c r="G77">
+        <f>1.96*G76</f>
+        <v>0.0012956791986519</v>
+      </c>
+      <c r="H77">
+        <f>Experiment!F41-H41</f>
+        <v>-4.89002741167338e-5</v>
+      </c>
+    </row>
+    <row r="78" customHeight="1" spans="1:7">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B78">
         <f>0.5-B77</f>
         <v>0.498820392149023</v>
       </c>
-    </row>
-    <row r="79" customHeight="1" spans="1:2">
+      <c r="F78" t="s">
+        <v>67</v>
+      </c>
+      <c r="G78">
+        <f>H77-G77</f>
+        <v>-0.00134457947276863</v>
+      </c>
+    </row>
+    <row r="79" customHeight="1" spans="1:7">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B79">
         <f>0.5+B77</f>
         <v>0.501179607850977</v>
       </c>
+      <c r="F79" t="s">
+        <v>68</v>
+      </c>
+      <c r="G79">
+        <f>H77+G77</f>
+        <v>0.00124677892453516</v>
+      </c>
     </row>
     <row r="82" customHeight="1" spans="1:1">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" customHeight="1" spans="1:2">
       <c r="A83" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B83">
         <f>SQRT(0.5*0.5/(C41+Experiment!C41))</f>
@@ -3071,7 +3286,7 @@
     </row>
     <row r="84" customHeight="1" spans="1:3">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B84">
         <f>1.96*B83</f>
@@ -3084,7 +3299,7 @@
     </row>
     <row r="85" customHeight="1" spans="1:2">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B85">
         <f>0.5-B84</f>
@@ -3093,7 +3308,7 @@
     </row>
     <row r="86" customHeight="1" spans="1:2">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B86">
         <f>0.5+B84</f>
@@ -3109,17 +3324,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" ht="12.75" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3135,10 +3350,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" spans="1:5">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>7716</v>
@@ -3152,10 +3370,14 @@
       <c r="E2" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" ht="12.75" spans="1:5">
+      <c r="F2">
+        <f>C2/B2</f>
+        <v>0.0889061689994816</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>9288</v>
@@ -3169,10 +3391,14 @@
       <c r="E3" s="2">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" ht="12.75" spans="1:5">
+      <c r="F3">
+        <f t="shared" ref="F3:F38" si="0">C3/B3</f>
+        <v>0.0845176571920758</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>10480</v>
@@ -3186,10 +3412,14 @@
       <c r="E4" s="2">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" ht="12.75" spans="1:5">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.0843511450381679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>9867</v>
@@ -3203,10 +3433,14 @@
       <c r="E5" s="2">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" ht="12.75" spans="1:5">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.083814735988649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>9793</v>
@@ -3220,10 +3454,14 @@
       <c r="E6" s="2">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" ht="12.75" spans="1:5">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.0849586439293373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>9500</v>
@@ -3237,10 +3475,14 @@
       <c r="E7" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" ht="12.75" spans="1:5">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.0829473684210526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>9088</v>
@@ -3254,10 +3496,14 @@
       <c r="E8" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" ht="12.75" spans="1:5">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.0858274647887324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>7664</v>
@@ -3271,10 +3517,14 @@
       <c r="E9" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" ht="12.75" spans="1:5">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.0850730688935282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>8434</v>
@@ -3288,10 +3538,14 @@
       <c r="E10" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" ht="12.75" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.0826416884040787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>10496</v>
@@ -3305,10 +3559,14 @@
       <c r="E11" s="2">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" ht="12.75" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.0819359756097561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>10551</v>
@@ -3322,10 +3580,14 @@
       <c r="E12" s="2">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" ht="12.75" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.0818879727040091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>9737</v>
@@ -3339,10 +3601,14 @@
       <c r="E13" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" ht="12.75" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.0822635308616617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>8176</v>
@@ -3356,10 +3622,14 @@
       <c r="E14" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" ht="12.75" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.0785225048923679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>9402</v>
@@ -3373,10 +3643,14 @@
       <c r="E15" s="2">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" ht="12.75" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.0741331631567752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <v>8669</v>
@@ -3390,10 +3664,14 @@
       <c r="E16" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" ht="12.75" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.0771715307417234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>8881</v>
@@ -3407,10 +3685,14 @@
       <c r="E17" s="2">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" ht="12.75" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.0780317531809481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>9655</v>
@@ -3424,10 +3706,14 @@
       <c r="E18" s="2">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" ht="12.75" spans="1:5">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.0798549974106681</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>9396</v>
@@ -3441,10 +3727,14 @@
       <c r="E19" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" ht="12.75" spans="1:5">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0.0783312047679864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>9262</v>
@@ -3458,10 +3748,14 @@
       <c r="E20" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" ht="12.75" spans="1:5">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.0784927661412222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
         <v>9308</v>
@@ -3475,10 +3769,14 @@
       <c r="E21" s="2">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" ht="12.75" spans="1:5">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.0782122905027933</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
         <v>8715</v>
@@ -3492,10 +3790,14 @@
       <c r="E22" s="2">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" ht="12.75" spans="1:5">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.0828456683878371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2">
         <v>8448</v>
@@ -3509,10 +3811,14 @@
       <c r="E23" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" ht="12.75" spans="1:5">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.0822679924242424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2">
         <v>8836</v>
@@ -3526,10 +3832,14 @@
       <c r="E24" s="2">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" ht="12.75" spans="1:5">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.0819375282933454</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>9359</v>
@@ -3539,10 +3849,14 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-    </row>
-    <row r="26" ht="12.75" spans="1:5">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.0843038786195106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>9427</v>
@@ -3552,10 +3866,14 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" ht="12.75" spans="1:5">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.0788161663307521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2">
         <v>9633</v>
@@ -3565,10 +3883,14 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" ht="12.75" spans="1:5">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.0838783348904806</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2">
         <v>9842</v>
@@ -3578,10 +3900,14 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" ht="12.75" spans="1:5">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.0844340581182687</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
         <v>9272</v>
@@ -3591,10 +3917,14 @@
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-    </row>
-    <row r="30" ht="12.75" spans="1:5">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.0827221742881795</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2">
         <v>8969</v>
@@ -3604,10 +3934,14 @@
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-    </row>
-    <row r="31" ht="12.75" spans="1:5">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.0847363139703423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2">
         <v>9697</v>
@@ -3617,10 +3951,14 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-    </row>
-    <row r="32" ht="12.75" spans="1:5">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.0876559760750748</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2">
         <v>10445</v>
@@ -3630,10 +3968,14 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-    </row>
-    <row r="33" ht="12.75" spans="1:5">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.0814743896601245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2">
         <v>9931</v>
@@ -3643,10 +3985,14 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" ht="12.75" spans="1:5">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.0836773738797704</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="2">
         <v>10042</v>
@@ -3656,10 +4002,14 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" ht="12.75" spans="1:5">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0.0798645688109938</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2">
         <v>9721</v>
@@ -3669,10 +4019,14 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-    </row>
-    <row r="36" ht="12.75" spans="1:5">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.0852792922538834</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2">
         <v>9304</v>
@@ -3682,10 +4036,14 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-    </row>
-    <row r="37" ht="12.75" spans="1:5">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.0827601031814273</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2">
         <v>8668</v>
@@ -3695,10 +4053,14 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" ht="12.75" spans="1:5">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0.0835256114443932</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2">
         <v>8988</v>
@@ -3708,10 +4070,14 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-    </row>
-    <row r="41" customHeight="1" spans="1:5">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0.0789942145082332</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:6">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <f>SUM(B2:B38)</f>
@@ -3728,6 +4094,10 @@
       <c r="E41">
         <f>SUM(E2:E24)</f>
         <v>1945</v>
+      </c>
+      <c r="F41">
+        <f>C2/B2</f>
+        <v>0.0889061689994816</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="3:3">

</xml_diff>

<commit_message>
Final project third upload
</commit_message>
<xml_diff>
--- a/p7/Final+Project+Results.xlsx
+++ b/p7/Final+Project+Results.xlsx
@@ -10,12 +10,15 @@
     <sheet name="Control" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Control!$A$1:$S$38</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
   <si>
     <t>Date</t>
   </si>
@@ -38,6 +41,9 @@
     <t>pay/click</t>
   </si>
   <si>
+    <t>pay/enroll</t>
+  </si>
+  <si>
     <t>Clicks/Pageviews</t>
   </si>
   <si>
@@ -51,6 +57,9 @@
   </si>
   <si>
     <t>B1-A1</t>
+  </si>
+  <si>
+    <t>b1-a1</t>
   </si>
   <si>
     <t>Sat, Oct 11</t>
@@ -236,9 +245,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,6 +268,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -266,36 +290,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -310,34 +322,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,24 +372,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,20 +418,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -419,7 +428,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,7 +446,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,31 +506,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,31 +578,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,85 +602,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,6 +619,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -624,6 +642,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,8 +673,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,24 +690,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,148 +722,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1181,17 +1190,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
+      <selection pane="bottomLeft" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1217,19 +1226,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
@@ -1240,10 +1249,19 @@
       <c r="P1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>7723</v>
@@ -1266,37 +1284,49 @@
         <v>0.101892285298399</v>
       </c>
       <c r="H2" s="1">
+        <f>E2/D2</f>
+        <v>0.522388059701492</v>
+      </c>
+      <c r="I2" s="1">
         <f>C2/B2</f>
         <v>0.0889550692735983</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>7716</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>686</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>105</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>34</v>
       </c>
-      <c r="M2">
-        <f>K2/J2</f>
+      <c r="N2">
+        <f>L2/K2</f>
         <v>0.153061224489796</v>
       </c>
-      <c r="N2">
-        <f>M2-F2</f>
+      <c r="O2">
+        <f>N2-F2</f>
         <v>-0.0419897216528531</v>
       </c>
-      <c r="O2">
-        <f>L2/J2</f>
+      <c r="P2">
+        <f>M2/K2</f>
         <v>0.0495626822157434</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="R2">
+        <f>M2/L2</f>
+        <v>0.323809523809524</v>
+      </c>
+      <c r="S2">
+        <f>R2-H2</f>
+        <v>-0.198578535891969</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>9102</v>
@@ -1319,37 +1349,49 @@
         <v>0.0898587933247754</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H38" si="2">C3/B3</f>
+        <f t="shared" ref="H3:H24" si="2">E3/D3</f>
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I38" si="3">C3/B3</f>
         <v>0.0855855855855856</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>9288</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>785</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>116</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>91</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M24" si="3">K3/J3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N24" si="4">L3/K3</f>
         <v>0.147770700636943</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N24" si="4">M3-F3</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O24" si="5">N3-F3</f>
         <v>-0.0409327653450853</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O24" si="5">L3/J3</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P24" si="6">M3/K3</f>
         <v>0.115923566878981</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="R3">
+        <f t="shared" ref="R3:R24" si="7">M3/L3</f>
+        <v>0.78448275862069</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S24" si="8">R3-H3</f>
+        <v>0.308292282430213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>10511</v>
@@ -1373,36 +1415,48 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" si="2"/>
+        <v>0.568862275449102</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="3"/>
         <v>0.0864808296070783</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>10480</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>884</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>145</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>79</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>0.164027149321267</v>
       </c>
       <c r="N4">
         <f t="shared" si="4"/>
-        <v>-0.019691222515917</v>
+        <v>0.164027149321267</v>
       </c>
       <c r="O4">
         <f t="shared" si="5"/>
+        <v>-0.019691222515917</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="6"/>
         <v>0.0893665158371041</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="R4">
+        <f t="shared" si="7"/>
+        <v>0.544827586206897</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="8"/>
+        <v>-0.0240346892422053</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>9871</v>
@@ -1426,40 +1480,52 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
+        <v>0.673076923076923</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="3"/>
         <v>0.0846925336845304</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>9867</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>827</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>138</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>92</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>0.166868198307134</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>-0.0197346725062628</v>
+        <v>0.166868198307134</v>
       </c>
       <c r="O5">
         <f t="shared" si="5"/>
+        <v>-0.0197346725062628</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
         <v>0.111245465538089</v>
       </c>
-      <c r="P5">
-        <f>O2-G2</f>
+      <c r="Q5">
+        <f>P2-G2</f>
         <v>-0.0523296030826556</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="R5">
+        <f t="shared" si="7"/>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="8"/>
+        <v>-0.0064102564102565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>10014</v>
@@ -1483,40 +1549,52 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
+        <v>0.392638036809816</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="3"/>
         <v>0.0835829838226483</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>9793</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>832</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>140</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>94</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>0.168269230769231</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>-0.0264738994577702</v>
+        <v>0.168269230769231</v>
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
+        <v>-0.0264738994577702</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
         <v>0.112980769230769</v>
       </c>
-      <c r="P6">
-        <f t="shared" ref="P6:P24" si="6">O3-G3</f>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q24" si="9">P3-G3</f>
         <v>0.0260647735542055</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="R6">
+        <f t="shared" si="7"/>
+        <v>0.671428571428571</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="8"/>
+        <v>0.278790534618755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>9670</v>
@@ -1540,40 +1618,52 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
+        <v>0.594202898550725</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="3"/>
         <v>0.0851085832471562</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>9500</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>788</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>129</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>61</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>0.163705583756345</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>-0.00397363860088484</v>
+        <v>0.163705583756345</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>0.0774111675126904</v>
+        <v>-0.00397363860088484</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
+        <v>0.0774111675126904</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="9"/>
         <v>-0.0151439352080009</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="R7">
+        <f t="shared" si="7"/>
+        <v>0.472868217054264</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="8"/>
+        <v>-0.121334681496461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>9008</v>
@@ -1597,40 +1687,52 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
+        <v>0.520547945205479</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="3"/>
         <v>0.0830373001776199</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>9088</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>780</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>127</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>44</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>0.162820512820513</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
-        <v>-0.0323666529548882</v>
+        <v>0.162820512820513</v>
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>0.0564102564102564</v>
+        <v>-0.0323666529548882</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
+        <v>0.0564102564102564</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="9"/>
         <v>-0.0143526205863125</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="R8">
+        <f t="shared" si="7"/>
+        <v>0.346456692913386</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="8"/>
+        <v>-0.174091252292094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>7434</v>
@@ -1654,40 +1756,52 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="2"/>
+        <v>0.636363636363636</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="3"/>
         <v>0.0850147968792037</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>7664</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>652</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>94</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>62</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>0.144171779141104</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>-0.0298788537702877</v>
+        <v>0.144171779141104</v>
       </c>
       <c r="O9">
         <f t="shared" si="5"/>
-        <v>0.0950920245398773</v>
+        <v>-0.0298788537702877</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
+        <v>0.0950920245398773</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="9"/>
         <v>0.0365172088962411</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="R9">
+        <f t="shared" si="7"/>
+        <v>0.659574468085106</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="8"/>
+        <v>0.02321083172147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2">
         <v>8459</v>
@@ -1711,40 +1825,52 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="2"/>
+        <v>0.458015267175573</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="3"/>
         <v>0.0816881428064783</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>8434</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>697</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>120</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>77</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>0.172166427546628</v>
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>-0.0174138908325326</v>
+        <v>0.172166427546628</v>
       </c>
       <c r="O10">
         <f t="shared" si="5"/>
-        <v>0.110473457675753</v>
+        <v>-0.0174138908325326</v>
       </c>
       <c r="P10">
         <f t="shared" si="6"/>
+        <v>0.110473457675753</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="9"/>
         <v>-0.0222243124387069</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="R10">
+        <f t="shared" si="7"/>
+        <v>0.641666666666667</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="8"/>
+        <v>0.183651399491094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2">
         <v>10667</v>
@@ -1768,40 +1894,52 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="2"/>
+        <v>0.587878787878788</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="3"/>
         <v>0.0807162276178869</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>10496</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>860</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>153</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>98</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>0.177906976744186</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>-0.013730653917835</v>
+        <v>0.177906976744186</v>
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
-        <v>0.113953488372093</v>
+        <v>-0.013730653917835</v>
       </c>
       <c r="P11">
         <f t="shared" si="6"/>
+        <v>0.113953488372093</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="9"/>
         <v>-0.0451940216646096</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="R11">
+        <f t="shared" si="7"/>
+        <v>0.640522875816993</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="8"/>
+        <v>0.0526440879382055</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>10660</v>
@@ -1825,40 +1963,52 @@
       </c>
       <c r="H12" s="1">
         <f t="shared" si="2"/>
+        <v>0.535714285714286</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="3"/>
         <v>0.0813320825515947</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>10551</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>864</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>143</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>71</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>0.165509259259259</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>-0.0605576380879147</v>
+        <v>0.165509259259259</v>
       </c>
       <c r="O12">
         <f t="shared" si="5"/>
-        <v>0.0821759259259259</v>
+        <v>-0.0605576380879147</v>
       </c>
       <c r="P12">
         <f t="shared" si="6"/>
+        <v>0.0821759259259259</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="9"/>
         <v>-0.0156674691310087</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="R12">
+        <f t="shared" si="7"/>
+        <v>0.496503496503497</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="8"/>
+        <v>-0.0392107892107892</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <v>9947</v>
@@ -1882,40 +2032,52 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="2"/>
+        <v>0.567901234567901</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="3"/>
         <v>0.0842465064843671</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>9737</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>801</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>128</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>70</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>0.15980024968789</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>-0.0335171727464779</v>
+        <v>0.15980024968789</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0.0873907615480649</v>
+        <v>-0.0335171727464779</v>
       </c>
       <c r="P13">
         <f t="shared" si="6"/>
+        <v>0.0873907615480649</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="9"/>
         <v>0.0236427775020918</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="R13">
+        <f t="shared" si="7"/>
+        <v>0.546875</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="8"/>
+        <v>-0.0210262345679012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2">
         <v>8324</v>
@@ -1939,40 +2101,52 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="2"/>
+        <v>0.440944881889764</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="3"/>
         <v>0.079889476213359</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>8176</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>642</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>122</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>68</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>0.190031152647975</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>-0.000946290961047924</v>
+        <v>0.190031152647975</v>
       </c>
       <c r="O14">
         <f t="shared" si="5"/>
-        <v>0.105919003115265</v>
+        <v>-0.000946290961047924</v>
       </c>
       <c r="P14">
         <f t="shared" si="6"/>
+        <v>0.105919003115265</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="9"/>
         <v>0.00129379034654103</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="R14">
+        <f t="shared" si="7"/>
+        <v>0.557377049180328</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="8"/>
+        <v>0.116432167290564</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
         <v>9434</v>
@@ -1996,40 +2170,52 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="2"/>
+        <v>0.554545454545455</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="3"/>
         <v>0.0713377146491414</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>9402</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>697</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>194</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>94</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="3"/>
-        <v>0.278335724533716</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>-0.0485587776951101</v>
+        <v>0.278335724533716</v>
       </c>
       <c r="O15">
         <f t="shared" si="5"/>
-        <v>0.134863701578192</v>
+        <v>-0.0485587776951101</v>
       </c>
       <c r="P15">
         <f t="shared" si="6"/>
+        <v>0.134863701578192</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="9"/>
         <v>-0.0389313405100601</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="R15">
+        <f t="shared" si="7"/>
+        <v>0.484536082474227</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="8"/>
+        <v>-0.0700093720712278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>8687</v>
@@ -2053,40 +2239,52 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
+        <v>0.727272727272727</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="3"/>
         <v>0.0795441464256936</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>8669</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>669</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>127</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>81</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
-        <v>0.1898355754858</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>-0.0648677530236073</v>
+        <v>0.1898355754858</v>
       </c>
       <c r="O16">
         <f t="shared" si="5"/>
-        <v>0.121076233183857</v>
+        <v>-0.0648677530236073</v>
       </c>
       <c r="P16">
         <f t="shared" si="6"/>
+        <v>0.121076233183857</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="9"/>
         <v>-0.0223944413158971</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="R16">
+        <f t="shared" si="7"/>
+        <v>0.637795275590551</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="8"/>
+        <v>-0.0894774516821761</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
         <v>8896</v>
@@ -2110,40 +2308,52 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" si="2"/>
+        <v>0.645962732919255</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
         <v>0.0795863309352518</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>8881</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>693</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>153</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>101</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="3"/>
-        <v>0.220779220779221</v>
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>-0.00662190916428224</v>
+        <v>0.220779220779221</v>
       </c>
       <c r="O17">
         <f t="shared" si="5"/>
-        <v>0.145743145743146</v>
+        <v>-0.00662190916428224</v>
       </c>
       <c r="P17">
         <f t="shared" si="6"/>
+        <v>0.145743145743146</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="9"/>
         <v>0.0217084767994753</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="R17">
+        <f t="shared" si="7"/>
+        <v>0.660130718954248</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="8"/>
+        <v>0.0141679860349937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
         <v>9535</v>
@@ -2167,40 +2377,52 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" si="2"/>
+        <v>0.532188841201717</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="3"/>
         <v>0.0796014682747771</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>9655</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>771</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>213</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>119</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>0.276264591439689</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>-0.0307182807605743</v>
+        <v>0.276264591439689</v>
       </c>
       <c r="O18">
         <f t="shared" si="5"/>
-        <v>0.154345006485084</v>
+        <v>-0.0307182807605743</v>
       </c>
       <c r="P18">
         <f t="shared" si="6"/>
+        <v>0.154345006485084</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="9"/>
         <v>-0.0464141587487018</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="R18">
+        <f t="shared" si="7"/>
+        <v>0.55868544600939</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="8"/>
+        <v>0.0264966048076729</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2">
         <v>9363</v>
@@ -2224,40 +2446,52 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="2"/>
+        <v>0.590909090909091</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="3"/>
         <v>0.0786072839901741</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>9396</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>736</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>162</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M19" s="2">
         <v>120</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="3"/>
-        <v>0.220108695652174</v>
       </c>
       <c r="N19">
         <f t="shared" si="4"/>
-        <v>0.0108695652173909</v>
+        <v>0.220108695652174</v>
       </c>
       <c r="O19">
         <f t="shared" si="5"/>
-        <v>0.16304347826087</v>
+        <v>0.0108695652173909</v>
       </c>
       <c r="P19">
         <f t="shared" si="6"/>
+        <v>0.16304347826087</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="9"/>
         <v>-0.0641625511866215</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="R19">
+        <f t="shared" si="7"/>
+        <v>0.740740740740741</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="8"/>
+        <v>0.14983164983165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2">
         <v>9327</v>
@@ -2281,40 +2515,52 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
+        <v>0.438775510204082</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
         <v>0.0792323362281548</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>9262</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>727</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>201</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>96</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="3"/>
-        <v>0.276478679504814</v>
       </c>
       <c r="N20">
         <f t="shared" si="4"/>
-        <v>0.0112554048092793</v>
+        <v>0.276478679504814</v>
       </c>
       <c r="O20">
         <f t="shared" si="5"/>
-        <v>0.132049518569464</v>
+        <v>0.0112554048092793</v>
       </c>
       <c r="P20">
         <f t="shared" si="6"/>
+        <v>0.132049518569464</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="9"/>
         <v>-0.00114950962408628</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="R20">
+        <f t="shared" si="7"/>
+        <v>0.477611940298507</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="8"/>
+        <v>0.0388364300944258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2">
         <v>9345</v>
@@ -2338,40 +2584,52 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" si="2"/>
+        <v>0.449101796407186</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
         <v>0.0785446762974853</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>9308</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>728</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>207</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>67</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="3"/>
-        <v>0.284340659340659</v>
       </c>
       <c r="N21">
         <f t="shared" si="4"/>
-        <v>0.0568202233733573</v>
+        <v>0.284340659340659</v>
       </c>
       <c r="O21">
         <f t="shared" si="5"/>
-        <v>0.092032967032967</v>
+        <v>0.0568202233733573</v>
       </c>
       <c r="P21">
         <f t="shared" si="6"/>
+        <v>0.092032967032967</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="9"/>
         <v>-0.0090278525399487</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="R21">
+        <f t="shared" si="7"/>
+        <v>0.323671497584541</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="8"/>
+        <v>-0.125430298822645</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2">
         <v>8890</v>
@@ -2395,40 +2653,52 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="2"/>
+        <v>0.580459770114943</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
         <v>0.0794150731158605</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>8715</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>722</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>182</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>123</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>0.25207756232687</v>
       </c>
       <c r="N22">
         <f t="shared" si="4"/>
-        <v>0.00561863881412178</v>
+        <v>0.25207756232687</v>
       </c>
       <c r="O22">
         <f t="shared" si="5"/>
-        <v>0.170360110803324</v>
+        <v>0.00561863881412178</v>
       </c>
       <c r="P22">
         <f t="shared" si="6"/>
+        <v>0.170360110803324</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="9"/>
         <v>0.0394021739130436</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="R22">
+        <f t="shared" si="7"/>
+        <v>0.675824175824176</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="8"/>
+        <v>0.0953644057092333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2">
         <v>8460</v>
@@ -2452,40 +2722,52 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" si="2"/>
+        <v>0.596153846153846</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
         <v>0.0804964539007092</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>8448</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>695</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>142</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>100</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="3"/>
-        <v>0.20431654676259</v>
       </c>
       <c r="N23">
         <f t="shared" si="4"/>
-        <v>-0.0247583431052511</v>
+        <v>0.20431654676259</v>
       </c>
       <c r="O23">
         <f t="shared" si="5"/>
-        <v>0.143884892086331</v>
+        <v>-0.0247583431052511</v>
       </c>
       <c r="P23">
         <f t="shared" si="6"/>
+        <v>0.143884892086331</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="9"/>
         <v>0.0156760408969335</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="R23">
+        <f t="shared" si="7"/>
+        <v>0.704225352112676</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="8"/>
+        <v>0.10807150595883</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2">
         <v>8836</v>
@@ -2509,40 +2791,52 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" si="2"/>
+        <v>0.325242718446602</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="3"/>
         <v>0.0784291534631055</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>8836</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>724</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>182</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>103</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="3"/>
-        <v>0.251381215469613</v>
       </c>
       <c r="N24">
         <f t="shared" si="4"/>
-        <v>-0.0458770817886837</v>
+        <v>0.251381215469613</v>
       </c>
       <c r="O24">
         <f t="shared" si="5"/>
-        <v>0.142265193370166</v>
+        <v>-0.0458770817886837</v>
       </c>
       <c r="P24">
         <f t="shared" si="6"/>
+        <v>0.142265193370166</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="9"/>
         <v>-0.010146869479295</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="R24">
+        <f t="shared" si="7"/>
+        <v>0.565934065934066</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="8"/>
+        <v>0.240691347487464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2">
         <v>9437</v>
@@ -2553,22 +2847,23 @@
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1">
-        <f t="shared" si="2"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1">
+        <f t="shared" si="3"/>
         <v>0.0835011126417294</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>9359</v>
       </c>
-      <c r="J25" s="2">
+      <c r="K25" s="2">
         <v>789</v>
       </c>
-      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2">
         <v>9420</v>
@@ -2579,22 +2874,23 @@
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1">
-        <f t="shared" si="2"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1">
+        <f t="shared" si="3"/>
         <v>0.0829087048832272</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>9427</v>
       </c>
-      <c r="J26" s="2">
+      <c r="K26" s="2">
         <v>743</v>
       </c>
-      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2">
         <v>9570</v>
@@ -2605,31 +2901,32 @@
       <c r="D27" s="1"/>
       <c r="E27" s="3"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1">
-        <f t="shared" si="2"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1">
+        <f t="shared" si="3"/>
         <v>0.0841170323928945</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>9633</v>
       </c>
-      <c r="J27" s="2">
+      <c r="K27" s="2">
         <v>808</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M27" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27">
-        <f>AVERAGE(N2:N24)</f>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27">
+        <f>AVERAGE(O2:O24)</f>
         <v>-0.0207845820292659</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2">
         <v>9921</v>
@@ -2640,29 +2937,30 @@
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1">
-        <f t="shared" si="2"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1">
+        <f t="shared" si="3"/>
         <v>0.083660921278097</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>9842</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>831</v>
       </c>
-      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" t="s">
-        <v>41</v>
-      </c>
-      <c r="N28">
-        <f>STDEV(N2:N24)</f>
+      <c r="M28" s="3"/>
+      <c r="N28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O28">
+        <f>STDEV(O2:O24)</f>
         <v>0.0269646409706782</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2">
         <v>9424</v>
@@ -2673,29 +2971,30 @@
       <c r="D29" s="1"/>
       <c r="E29" s="3"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1">
-        <f t="shared" si="2"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1">
+        <f t="shared" si="3"/>
         <v>0.0828735144312394</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>9272</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>767</v>
       </c>
-      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" t="s">
-        <v>43</v>
-      </c>
-      <c r="N29">
-        <f>1.96*N28</f>
+      <c r="M29" s="3"/>
+      <c r="N29" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29">
+        <f>1.96*O28</f>
         <v>0.0528506963025294</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2">
         <v>9010</v>
@@ -2706,29 +3005,30 @@
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1">
-        <f t="shared" si="2"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1">
+        <f t="shared" si="3"/>
         <v>0.0839067702552719</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>8969</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>760</v>
       </c>
-      <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" t="s">
-        <v>45</v>
-      </c>
-      <c r="N30">
-        <f>N27-N29</f>
+      <c r="M30" s="3"/>
+      <c r="N30" t="s">
+        <v>47</v>
+      </c>
+      <c r="O30">
+        <f>O27-O29</f>
         <v>-0.0736352783317953</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
         <v>9656</v>
@@ -2739,29 +3039,30 @@
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1">
-        <f t="shared" si="2"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1">
+        <f t="shared" si="3"/>
         <v>0.0854391052195526</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>9697</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>850</v>
       </c>
-      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" t="s">
-        <v>47</v>
-      </c>
-      <c r="N31">
-        <f>N27+N29</f>
+      <c r="M31" s="3"/>
+      <c r="N31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O31">
+        <f>O27+O29</f>
         <v>0.0320661142732634</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2">
         <v>10419</v>
@@ -2772,22 +3073,23 @@
       <c r="D32" s="1"/>
       <c r="E32" s="3"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1">
-        <f t="shared" si="2"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1">
+        <f t="shared" si="3"/>
         <v>0.0838852097130243</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>10445</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>851</v>
       </c>
-      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="2">
         <v>9880</v>
@@ -2798,22 +3100,23 @@
       <c r="D33" s="1"/>
       <c r="E33" s="3"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1">
-        <f t="shared" si="2"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1">
+        <f t="shared" si="3"/>
         <v>0.0840080971659919</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>9931</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>831</v>
       </c>
-      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="M33" s="3"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2">
         <v>10134</v>
@@ -2824,31 +3127,32 @@
       <c r="D34" s="1"/>
       <c r="E34" s="3"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1">
-        <f t="shared" si="2"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <f t="shared" si="3"/>
         <v>0.0790408525754885</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>10042</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>802</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M34" t="s">
-        <v>39</v>
-      </c>
-      <c r="N34">
-        <f>AVERAGE(P2:P24)</f>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N34" t="s">
+        <v>41</v>
+      </c>
+      <c r="O34">
+        <f>AVERAGE(Q2:Q24)</f>
         <v>-0.00964167218036863</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2">
         <v>9717</v>
@@ -2859,29 +3163,30 @@
       <c r="D35" s="1"/>
       <c r="E35" s="3"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1">
-        <f t="shared" si="2"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1">
+        <f t="shared" si="3"/>
         <v>0.0837707111248328</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>9721</v>
       </c>
-      <c r="J35" s="2">
+      <c r="K35" s="2">
         <v>829</v>
       </c>
-      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="M35" t="s">
-        <v>41</v>
-      </c>
-      <c r="N35">
-        <f>STDEV(P2:P24)</f>
+      <c r="M35" s="3"/>
+      <c r="N35" t="s">
+        <v>43</v>
+      </c>
+      <c r="O35">
+        <f>STDEV(Q2:Q24)</f>
         <v>0.0302737400577862</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B36" s="2">
         <v>9192</v>
@@ -2892,29 +3197,30 @@
       <c r="D36" s="1"/>
       <c r="E36" s="3"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1">
-        <f t="shared" si="2"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1">
+        <f t="shared" si="3"/>
         <v>0.0799608355091384</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>9304</v>
       </c>
-      <c r="J36" s="2">
+      <c r="K36" s="2">
         <v>770</v>
       </c>
-      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" t="s">
-        <v>43</v>
-      </c>
-      <c r="N36">
-        <f>1.96*N35</f>
+      <c r="M36" s="3"/>
+      <c r="N36" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36">
+        <f>1.96*O35</f>
         <v>0.059336530513261</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B37" s="2">
         <v>8630</v>
@@ -2925,29 +3231,30 @@
       <c r="D37" s="1"/>
       <c r="E37" s="3"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1">
-        <f t="shared" si="2"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1">
+        <f t="shared" si="3"/>
         <v>0.0860950173812283</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>8668</v>
       </c>
-      <c r="J37" s="2">
+      <c r="K37" s="2">
         <v>724</v>
       </c>
-      <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="M37" t="s">
-        <v>45</v>
-      </c>
-      <c r="N37">
-        <f>N34-N35</f>
+      <c r="M37" s="3"/>
+      <c r="N37" t="s">
+        <v>47</v>
+      </c>
+      <c r="O37">
+        <f>O34-O35</f>
         <v>-0.0399154122381548</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B38" s="2">
         <v>8970</v>
@@ -2958,23 +3265,24 @@
       <c r="D38" s="1"/>
       <c r="E38" s="3"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1">
-        <f t="shared" si="2"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1">
+        <f t="shared" si="3"/>
         <v>0.0804905239687848</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>8988</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>710</v>
       </c>
-      <c r="K38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="M38" t="s">
-        <v>47</v>
-      </c>
-      <c r="N38">
-        <f>N34+N35</f>
+      <c r="M38" s="3"/>
+      <c r="N38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O38">
+        <f>O34+O35</f>
         <v>0.0206320678774176</v>
       </c>
     </row>
@@ -2992,9 +3300,9 @@
       <c r="D40" s="1"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" customHeight="1" spans="1:8">
+    <row r="41" customHeight="1" spans="1:9">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B41">
         <f>SUM(B2:B38)</f>
@@ -3012,14 +3320,14 @@
         <f>SUM(E2:E24)</f>
         <v>2033</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <f>C2/B2</f>
         <v>0.0889550692735983</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="2:3">
       <c r="B42" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C42">
         <f>SUM(C2:C24)</f>
@@ -3028,7 +3336,7 @@
     </row>
     <row r="43" customHeight="1" spans="2:3">
       <c r="B43" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <f>(D41+Experiment!D41)/(C42+Experiment!C42)</f>
@@ -3037,7 +3345,7 @@
     </row>
     <row r="44" customHeight="1" spans="2:3">
       <c r="B44" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <f>SQRT(C43*(1-C43)*(1/C42+1/Experiment!C42))</f>
@@ -3046,7 +3354,7 @@
     </row>
     <row r="45" customHeight="1" spans="2:3">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <f>1.96*C44</f>
@@ -3055,7 +3363,7 @@
     </row>
     <row r="46" customHeight="1" spans="2:3">
       <c r="B46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <f>G47-C45</f>
@@ -3064,14 +3372,14 @@
     </row>
     <row r="47" customHeight="1" spans="2:7">
       <c r="B47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <f>G47+C45</f>
         <v>-0.0119863908253187</v>
       </c>
       <c r="F47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G47">
         <f>3423/17260-3785/17293</f>
@@ -3080,14 +3388,14 @@
     </row>
     <row r="50" customHeight="1" spans="2:7">
       <c r="B50" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C50">
         <f>(E41+Experiment!E41)/(C42+Experiment!C42)</f>
         <v>0.115127485312419</v>
       </c>
       <c r="F50" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G50">
         <f>1945/17260-2033/17293</f>
@@ -3096,7 +3404,7 @@
     </row>
     <row r="51" customHeight="1" spans="2:3">
       <c r="B51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C51">
         <f>SQRT(C50*(1-C50)*(1/C42+1/Experiment!C42))</f>
@@ -3105,7 +3413,7 @@
     </row>
     <row r="52" customHeight="1" spans="2:3">
       <c r="B52" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C52">
         <f>1.96*C51</f>
@@ -3114,7 +3422,7 @@
     </row>
     <row r="53" customHeight="1" spans="2:3">
       <c r="B53" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C53">
         <f>G50-C52</f>
@@ -3123,7 +3431,7 @@
     </row>
     <row r="54" customHeight="1" spans="2:3">
       <c r="B54" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C54">
         <f>G50+C52</f>
@@ -3132,7 +3440,7 @@
     </row>
     <row r="56" customHeight="1" spans="2:3">
       <c r="B56" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <f>(E41+Experiment!E41)/(D41+Experiment!D41)</f>
@@ -3141,7 +3449,7 @@
     </row>
     <row r="57" customHeight="1" spans="2:3">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C57">
         <f>SQRT(C56*(1-C56)*(1/D41+1/Experiment!D41))</f>
@@ -3150,7 +3458,7 @@
     </row>
     <row r="58" customHeight="1" spans="2:3">
       <c r="B58" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <f>1.96*C57</f>
@@ -3159,7 +3467,7 @@
     </row>
     <row r="59" customHeight="1" spans="2:3">
       <c r="B59" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C59">
         <f>G50-C58</f>
@@ -3168,30 +3476,30 @@
     </row>
     <row r="60" customHeight="1" spans="2:3">
       <c r="B60" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C60">
         <f>G50+C58</f>
         <v>0.0181166463045786</v>
       </c>
     </row>
-    <row r="74" customHeight="1" spans="6:8">
+    <row r="74" customHeight="1" spans="6:9">
       <c r="F74" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H74" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="I74" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="75" customHeight="1" spans="1:7">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F75" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G75">
         <f>(C41+Experiment!C41)/(B41+Experiment!B41)</f>
@@ -3200,23 +3508,23 @@
     </row>
     <row r="76" customHeight="1" spans="1:7">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B76">
         <f>SQRT(0.5*0.5/(B41+344660))</f>
         <v>0.000601840740294325</v>
       </c>
       <c r="F76" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G76">
         <f>SQRT(G75*(1-G75)*(1/B41+1/Experiment!B41))</f>
         <v>0.000661060815638722</v>
       </c>
     </row>
-    <row r="77" customHeight="1" spans="1:8">
+    <row r="77" customHeight="1" spans="1:9">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B77">
         <f>1.96*B76</f>
@@ -3227,57 +3535,57 @@
         <v>0.500639666880613</v>
       </c>
       <c r="F77" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G77">
         <f>1.96*G76</f>
         <v>0.0012956791986519</v>
       </c>
-      <c r="H77">
-        <f>Experiment!F41-H41</f>
-        <v>-4.89002741167338e-5</v>
+      <c r="I77">
+        <f>Experiment!F41-I41</f>
+        <v>-4.89002741166922e-5</v>
       </c>
     </row>
     <row r="78" customHeight="1" spans="1:7">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B78">
         <f>0.5-B77</f>
         <v>0.498820392149023</v>
       </c>
       <c r="F78" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G78">
-        <f>H77-G77</f>
-        <v>-0.00134457947276863</v>
+        <f>I77-G77</f>
+        <v>-0.00134457947276859</v>
       </c>
     </row>
     <row r="79" customHeight="1" spans="1:7">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B79">
         <f>0.5+B77</f>
         <v>0.501179607850977</v>
       </c>
       <c r="F79" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G79">
-        <f>H77+G77</f>
-        <v>0.00124677892453516</v>
+        <f>I77+G77</f>
+        <v>0.00124677892453521</v>
       </c>
     </row>
     <row r="82" customHeight="1" spans="1:1">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" customHeight="1" spans="1:2">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B83">
         <f>SQRT(0.5*0.5/(C41+Experiment!C41))</f>
@@ -3286,7 +3594,7 @@
     </row>
     <row r="84" customHeight="1" spans="1:3">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B84">
         <f>1.96*B83</f>
@@ -3299,7 +3607,7 @@
     </row>
     <row r="85" customHeight="1" spans="1:2">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B85">
         <f>0.5-B84</f>
@@ -3308,7 +3616,7 @@
     </row>
     <row r="86" customHeight="1" spans="1:2">
       <c r="A86" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B86">
         <f>0.5+B84</f>
@@ -3316,6 +3624,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S38"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -3334,7 +3643,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" ht="12.75" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3351,12 +3660,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="12.75" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>7716</v>
@@ -3375,9 +3684,9 @@
         <v>0.0889061689994816</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="12.75" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>9288</v>
@@ -3396,9 +3705,9 @@
         <v>0.0845176571920758</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="12.75" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>10480</v>
@@ -3417,9 +3726,9 @@
         <v>0.0843511450381679</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" ht="12.75" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>9867</v>
@@ -3438,9 +3747,9 @@
         <v>0.083814735988649</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" ht="12.75" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>9793</v>
@@ -3459,9 +3768,9 @@
         <v>0.0849586439293373</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" ht="12.75" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>9500</v>
@@ -3480,9 +3789,9 @@
         <v>0.0829473684210526</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" ht="12.75" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>9088</v>
@@ -3501,9 +3810,9 @@
         <v>0.0858274647887324</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" ht="12.75" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>7664</v>
@@ -3522,9 +3831,9 @@
         <v>0.0850730688935282</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" ht="12.75" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2">
         <v>8434</v>
@@ -3543,9 +3852,9 @@
         <v>0.0826416884040787</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" ht="12.75" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2">
         <v>10496</v>
@@ -3564,9 +3873,9 @@
         <v>0.0819359756097561</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" ht="12.75" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>10551</v>
@@ -3585,9 +3894,9 @@
         <v>0.0818879727040091</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" ht="12.75" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <v>9737</v>
@@ -3606,9 +3915,9 @@
         <v>0.0822635308616617</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" ht="12.75" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2">
         <v>8176</v>
@@ -3627,9 +3936,9 @@
         <v>0.0785225048923679</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" ht="12.75" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
         <v>9402</v>
@@ -3648,9 +3957,9 @@
         <v>0.0741331631567752</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" ht="12.75" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>8669</v>
@@ -3669,9 +3978,9 @@
         <v>0.0771715307417234</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" ht="12.75" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
         <v>8881</v>
@@ -3690,9 +3999,9 @@
         <v>0.0780317531809481</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" ht="12.75" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
         <v>9655</v>
@@ -3711,9 +4020,9 @@
         <v>0.0798549974106681</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" ht="12.75" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2">
         <v>9396</v>
@@ -3732,9 +4041,9 @@
         <v>0.0783312047679864</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" ht="12.75" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2">
         <v>9262</v>
@@ -3753,9 +4062,9 @@
         <v>0.0784927661412222</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" ht="12.75" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2">
         <v>9308</v>
@@ -3774,9 +4083,9 @@
         <v>0.0782122905027933</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" ht="12.75" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2">
         <v>8715</v>
@@ -3795,9 +4104,9 @@
         <v>0.0828456683878371</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" ht="12.75" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2">
         <v>8448</v>
@@ -3816,9 +4125,9 @@
         <v>0.0822679924242424</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" ht="12.75" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2">
         <v>8836</v>
@@ -3837,9 +4146,9 @@
         <v>0.0819375282933454</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" ht="12.75" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2">
         <v>9359</v>
@@ -3854,9 +4163,9 @@
         <v>0.0843038786195106</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" ht="12.75" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2">
         <v>9427</v>
@@ -3871,9 +4180,9 @@
         <v>0.0788161663307521</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" ht="12.75" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2">
         <v>9633</v>
@@ -3888,9 +4197,9 @@
         <v>0.0838783348904806</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" ht="12.75" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2">
         <v>9842</v>
@@ -3905,9 +4214,9 @@
         <v>0.0844340581182687</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" ht="12.75" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2">
         <v>9272</v>
@@ -3922,9 +4231,9 @@
         <v>0.0827221742881795</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" ht="12.75" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2">
         <v>8969</v>
@@ -3939,9 +4248,9 @@
         <v>0.0847363139703423</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" ht="12.75" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
         <v>9697</v>
@@ -3956,9 +4265,9 @@
         <v>0.0876559760750748</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" ht="12.75" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2">
         <v>10445</v>
@@ -3973,9 +4282,9 @@
         <v>0.0814743896601245</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" ht="12.75" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="2">
         <v>9931</v>
@@ -3990,9 +4299,9 @@
         <v>0.0836773738797704</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" ht="12.75" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2">
         <v>10042</v>
@@ -4007,9 +4316,9 @@
         <v>0.0798645688109938</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" ht="12.75" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2">
         <v>9721</v>
@@ -4024,9 +4333,9 @@
         <v>0.0852792922538834</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" ht="12.75" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B36" s="2">
         <v>9304</v>
@@ -4041,9 +4350,9 @@
         <v>0.0827601031814273</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" ht="12.75" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B37" s="2">
         <v>8668</v>
@@ -4058,9 +4367,9 @@
         <v>0.0835256114443932</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" ht="12.75" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B38" s="2">
         <v>8988</v>
@@ -4077,7 +4386,7 @@
     </row>
     <row r="41" customHeight="1" spans="1:6">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B41">
         <f>SUM(B2:B38)</f>

</xml_diff>